<commit_message>
Enhancing eMoF creation to be more flexible, and now accounts for special characters in units
</commit_message>
<xml_diff>
--- a/raw-v3/eMoF Fields edna2obis .xlsx
+++ b/raw-v3/eMoF Fields edna2obis .xlsx
@@ -84,7 +84,7 @@
 Field type: numeric</t>
       </text>
     </comment>
-    <comment authorId="0" ref="C15">
+    <comment authorId="0" ref="E15">
       <text>
         <t xml:space="preserve">Requirement level: Optional
 Description: Unit for pump_flow_rate
@@ -122,6 +122,68 @@
 Description: Description of method/instrument used for concentration measurement
 Example: Qubit 4.0 Fluorometer (Invitrogen)
 Field type: free text</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="A23">
+      <text>
+        <t xml:space="preserve">Requirement level: Highly recommended
+Description: Solution within which the sample was stored. Note: If a asample was processed before DNA extraction (e.g., filtration, homogenisation, subsampling), enter the storage solution before the process here, and the storage solution of the processed sample under the term prepped_samp_store_sol.
+Example: none
+Field type: controlled vocabulary (ethanol | sodium acetate | longmire | lysis buffer | none | other:)</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="A24">
+      <text>
+        <t xml:space="preserve">Requirement level: Highly recommended
+Description: Duration for which the sample was stored prior to DNA extraction, written in ISO 8601 format (i.e., P14D for 14 days period. P1Y6M for 1 year and 6 months period. P1W/4W for some time between 1 and 4 weeks). Note: If a sample was processed before DNA extraction (e.g., filtration, homogenisation, subsampling), enter the storage duration before the process here, and the storage duration of the processed sample under the term prepped_samp_store_temp.
+Example: P1Y6M
+Field type: fixed format (PnYnMnWnDTnHnMnS)</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="A25">
+      <text>
+        <t xml:space="preserve">Requirement level: Optional
+Description: Location at which extracted DNA was stored, usually name of a specific freezer/room
+Example: UWA, IOMRC, Lv4 -80Freezer2
+Field type: free text</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="A26">
+      <text>
+        <t xml:space="preserve">Requirement level: Optional
+Description: Additional information on sample storage method, that has not been shared in the given record.
+Example: The sample was thawed overnight at room temperature prior to DNA extraction
+Field type: free text</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="A27">
+      <text>
+        <t xml:space="preserve">Requirement level: Recommended
+Description: Duration of on-site, stationed sampling (i.e., the filter deployment period). This term is recommended to be recorded when filters are deployed directly in the environment, such as during airborne eDNA sampling or when filters are submerged in water for a certain period). The duration should be recorded using ISO 8601 duration format (P&lt;date&gt;T&lt;time&gt;). For example, P1Y1M1DT1H1M1.1S represents 1 year, 1 month, 1 day, 1 hour, 1 minute, 1 second, and 100 milliseconds
+Example: T1H30M
+Field type: fixed format (PnYnMnWnDTnHnMnS)</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="A28">
+      <text>
+        <t xml:space="preserve">Requirement level: Optional
+Description: Matiral used to pre-filter/pre-sort the sample
+Example: nylon
+Field type: free text</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="A29">
+      <text>
+        <t xml:space="preserve">Requirement level: Highly recommended
+Description: Refers to the mesh/pore size used to pre-filter/pre-sort the sample. Materials larger than the size threshold are excluded from the sample. Unit = µm
+Example: 20.0
+Field type: numeric</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="C1">
+      <text>
+        <t xml:space="preserve">Only for non-numeric, unique values that have a measurementValueID
+	-Katherine Silliman - NOAA Affiliate</t>
       </text>
     </comment>
     <comment authorId="0" ref="A1">
@@ -140,28 +202,16 @@
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A3">
-      <text>
-        <t xml:space="preserve">Requirement level: Recommended
-Description: Diameter of a filter if circular. Unit = mm
-Example: 47.0
-Field type: numeric</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="A1">
-      <text>
-        <t xml:space="preserve">Please correct me if im wrong, but from my understanding, there are not very many Occurrence linked measurements in metabarcoding data. Most of our measurements in the eMoF will be Event linked. I think there will be so few occurrence-specific measurements that we can hard code them like this. If we don't have this column, and fill in every eventID and occurrenceID row, our eMoF will grow exponentially large. So large in fact, that gomecc4 would come very close to the file length limit of Excel
-	-Bayden Willms - NOAA Affiliate
-Basically, you can summarize my above comment with this logic:  if the value is the same for all occurrences from that sample, it’s event; if it varies by taxon within that sample, it’s occurrence
-	-Bayden Willms - NOAA Affiliate
-Plus, any column that is in either DNA Derived Extension or the Occurrence Core should not be included in eMoF
-	-Bayden Willms - NOAA Affiliate</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="C4">
-      <text>
-        <t xml:space="preserve">need way to indicate 'this measurement unit is temperature_unit column in FAIRe checklist'
-	-Katherine Silliman - NOAA Affiliate</t>
+    <comment authorId="0" ref="F1">
+      <text>
+        <t xml:space="preserve">Also added this column to link to MixS ids.
+	-Brynn Zalmanek - NOAA Affiliate</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="G1">
+      <text>
+        <t xml:space="preserve">I added this column for now to add the closest related NERC term if I couldn't find one that fit exactly.
+	-Brynn Zalmanek - NOAA Affiliate</t>
       </text>
     </comment>
   </commentList>
@@ -174,6 +224,232 @@
     <author/>
   </authors>
   <commentList>
+    <comment authorId="0" ref="A5">
+      <text>
+        <t xml:space="preserve">Requirement level: Mandatory
+Description: A type/category of a sample. 'Sample" includes biological and technical replicates. If negative or positive control was selected, provide further infomration under the terms fill neg_cont_type and pos_cont_type.
+Example: sample
+Field type: controlled vocabulary (sample | negative control | positive control | PCR standard | other:)</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="A6">
+      <text>
+        <t xml:space="preserve">Requirement level: Recommended
+Description: Whether samples were taken from natural (0) or artificial (1) habitat. The examples of artificial habitat include mesocosm tank in lab, enclosure in zoo etc., including semi-natural systems. The definition of natural habitat is locations uncontrolled by researchers
+Example: 0
+Field type: Boolean</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="A7">
+      <text>
+        <t xml:space="preserve">Requirement level: Highly recommended
+Description: Temperature at which the sample was stored. Enter either the fixed term "ambient temperature" or a numeric value. Note: If a sample was processed before DNA extraction (e.g., filtration, homogenisation, subsampling), enter the storage temperature before the process here, and the storage temperature of the processed sample (i.e., filter paper) under a term prepped_samp_store_temp. Unit = degree Celsius
+Example: -80.0
+Field type: numeric or controlled vocabulary</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="A8">
+      <text>
+        <t xml:space="preserve">Requirement level: Highly recommended
+Description: Solution within which the sample was stored. Note: If a asample was processed before DNA extraction (e.g., filtration, homogenisation, subsampling), enter the storage solution before the process here, and the storage solution of the processed sample under the term prepped_samp_store_sol.
+Example: none
+Field type: controlled vocabulary (ethanol | sodium acetate | longmire | lysis buffer | none | other:)</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="A9">
+      <text>
+        <t xml:space="preserve">Requirement level: Highly recommended
+Description: Duration for which the sample was stored prior to DNA extraction, written in ISO 8601 format (i.e., P14D for 14 days period. P1Y6M for 1 year and 6 months period. P1W/4W for some time between 1 and 4 weeks). Note: If a sample was processed before DNA extraction (e.g., filtration, homogenisation, subsampling), enter the storage duration before the process here, and the storage duration of the processed sample under the term prepped_samp_store_temp.
+Example: P1Y6M
+Field type: fixed format (PnYnMnWnDTnHnMnS)</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="A10">
+      <text>
+        <t xml:space="preserve">Requirement level: Optional
+Description: Location at which sample was stored, usually name of a specific freezer/room
+Example: UWA, IOMRC, Lv4 -80Freezer1
+Field type: free text</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="A11">
+      <text>
+        <t xml:space="preserve">Requirement level: Optional
+Description: Location at which extracted DNA was stored, usually name of a specific freezer/room
+Example: UWA, IOMRC, Lv4 -80Freezer2
+Field type: free text</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="A12">
+      <text>
+        <t xml:space="preserve">Requirement level: Recommended
+Description: Whether water/ air samples were collected using active (i.e. pump, fan) or passive (i.e. submerged materials in water/air) filtration approach. Active = 1, Passive = 0
+Example: 1
+Field type: Boolean</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="A13">
+      <text>
+        <t xml:space="preserve">Requirement level: Recommended
+Description: Diameter of a filter if circular. Unit = mm
+Example: 47.0
+Field type: numeric</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="A14">
+      <text>
+        <t xml:space="preserve">Requirement level: Highly recommended
+Description: Material of filter
+Example: cellulose ester
+Field type: controlled vocabulary (cellulose | cellulose ester | glass fiber | thermoplastic membrane | track etched polycarbonate | nylon | polyethersulfone| other:)</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="A15">
+      <text>
+        <t xml:space="preserve">Requirement level: Recommended
+Description: Commercial names and brand of filter
+Example: Merck Sterivex
+Field type: free text</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="A16">
+      <text>
+        <t xml:space="preserve">Requirement level: Recommended
+Description: Temperature at which the prepared sample was stored prior to DNA extraction. Record either 'ambient' or a numeric value in degree Celsius. Note: The storage temprature of the original environmental sample (e.g., water, soil) should be recorded under samp_store_temp, while the current term is for the "processed" sample such as filter paper, homogenised and subsampled sediment, prepared for DNA extraction. Unit = degree Celsius
+Example: ambient temperature
+Field type: numeric or controlled vocabulary</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="A17">
+      <text>
+        <t xml:space="preserve">Requirement level: Recommended
+Description: Solution within which the prepared sample was stored prior to DNA extraction. Note: The storage solution of the original environmental sample (e.g., water, soil) should be recorded under samp_store_sol, while the current term is for the "processed" sample such as filter paper, homogenised and subsampled sediment, prepared for DNA extraction.
+Example: lysis buffer
+Field type: controlled vocabulary (ethanol | sodium acetate | longmire | lysis buffer | none | other:)</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="A18">
+      <text>
+        <t xml:space="preserve">Requirement level: Recommended
+Description: Duration for which the prepared sample was stored prior to DNA extraction, written in ISO 8601 format (i.e., P14D for 14 days period. P1Y6M for 1 year and 6 months period. P1W/4W for some time between 1 and 4 weeks). Note: The storage duration of the original environmental sample (e.g., water, soil) should be recorded under samp_store_dur, while the current term is for the "processed" sample such as filter paper, homogenised and subsampled sediment, prepared for DNA extraction.
+Example: P1Y6M
+Field type: fixed format (PnYnMnWnDTnHnMnS)</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="A19">
+      <text>
+        <t xml:space="preserve">Requirement level: Optional
+Description: Date of nucleic acid extraction, written in ISO 8601 format
+Example: 2008-01-23T19:23-06:00
+Field type: fixed format (nan)</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="A20">
+      <text>
+        <t xml:space="preserve">Requirement level: Recommended
+Description: The approach used to lyse DNA-containing material. For example, physical methods may involve freeze-thaw cycles or the uses of bead mills, homogenizers and sonicators. Thermal methods apply high temperatures, often used in combination wiht other methods.
+Example: enzymatic
+Field type: controlled vocabulary (physical | chemical | enzymatic | thermal | osmotic | other:)</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="A21">
+      <text>
+        <t xml:space="preserve">Requirement level: Recommended
+Description: The approach used to separate DNA from a mixture.
+Example: column-based
+Field type: controlled vocabulary (column-based | magnetic beads | centrifugation | precipitation | phenol chloroform | gel electrophoresis | other:)</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="A22">
+      <text>
+        <t xml:space="preserve">Requirement level: Highly recommended
+Description: The name of the extraction kit used to recover the nucleic acid fraction of an input material
+Example: Qiagen PowerSoil Kit
+Field type: free text</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="A23">
+      <text>
+        <t xml:space="preserve">Requirement level: Recommended
+Description: Was the extracted DNA cleaned/purified? Yes = 1, No =0
+Example: 1
+Field type: Boolean</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="A24">
+      <text>
+        <t xml:space="preserve">Requirement level: Recommended (If dna_cleanup_0_1 is 1)
+Description: A description of DNA clean-up method. Provide the name of a commercial kit if used.
+Example: Zymo DNA Clean &amp; Concentrator Kits
+Field type: free text</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="A25">
+      <text>
+        <t xml:space="preserve">Requirement level: Optional
+Description: Description of method/instrument used for concentration measurement
+Example: Qubit 4.0 Fluorometer (Invitrogen)
+Field type: free text</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="A27">
+      <text>
+        <t xml:space="preserve">Requirement level: Optional
+Description: Concentration of chlorophyll. Unit = mg/m3
+Example: 5.0
+Field type: numeric</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="E27">
+      <text>
+        <t xml:space="preserve">Requirement level: Optional
+Description: Concentration of chlorophyll. Unit = mg/m3
+Example: 5.0
+Field type: numeric</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="A28">
+      <text>
+        <t xml:space="preserve">Requirement level: Optional
+Description: The total concentration of all dissolved salts in a liquid or solid sample. While salinity can be measured by a complete chemical analysis, this method is difficult and time consuming. More often, it is instead derived from the conductivity measurement. This is known as practical salinity. These derivations compare the specific conductance of the sample to a salinity standard such as seawater. Unit = partical salinity unit (psu)
+Example: 25.0
+Field type: numeric</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="A29">
+      <text>
+        <t xml:space="preserve">Requirement level: Optional
+Description: Concentration of dissolved oxygen
+Example: 175.0
+Field type: numeric</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="B1">
+      <text>
+        <t xml:space="preserve">Please correct me if im wrong, but from my understanding, there are not very many Occurrence linked measurements in metabarcoding data. Most of our measurements in the eMoF will be Event linked. I think there will be so few occurrence-specific measurements that we can hard code them like this. If we don't have this column, and fill in every eventID and occurrenceID row, our eMoF will grow exponentially large. So large in fact, that gomecc4 would come very close to the file length limit of Excel
+	-Bayden Willms - NOAA Affiliate
+Basically, you can summarize my above comment with this logic:  if the value is the same for all occurrences from that sample, it’s event; if it varies by taxon within that sample, it’s occurrence
+	-Bayden Willms - NOAA Affiliate
+Plus, any column that is in either DNA Derived Extension or the Occurrence Core should not be included in eMoF
+	-Bayden Willms - NOAA Affiliate</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="D2">
+      <text>
+        <t xml:space="preserve">need way to indicate 'this measurement unit is temperature_unit column in FAIRe checklist'
+	-Katherine Silliman - NOAA Affiliate</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
     <comment authorId="0" ref="C4">
       <text>
         <t xml:space="preserve">Requirement level: Mandatory (Mandatory unless samp_category = negative control, positive control, or PCR standard)
@@ -219,7 +495,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="275">
   <si>
     <t>measurementType</t>
   </si>
@@ -227,12 +503,15 @@
     <t>measurementTypeID</t>
   </si>
   <si>
+    <t>measurementValue</t>
+  </si>
+  <si>
+    <t>measurementValueID</t>
+  </si>
+  <si>
     <t xml:space="preserve">measurementUnit </t>
   </si>
   <si>
-    <t>measurementUnit_column</t>
-  </si>
-  <si>
     <t>measurementUnitID</t>
   </si>
   <si>
@@ -242,15 +521,24 @@
     <t>temp</t>
   </si>
   <si>
+    <t>SDN:P07::CFSN0335</t>
+  </si>
+  <si>
     <t>degree Celsius</t>
   </si>
   <si>
+    <t>SDN:P06::UPAA</t>
+  </si>
+  <si>
     <t>samp_weather</t>
   </si>
   <si>
     <t>tot_depth_water_col</t>
   </si>
   <si>
+    <t>SDN:P07::CFV13N17</t>
+  </si>
+  <si>
     <t>elev</t>
   </si>
   <si>
@@ -305,9 +593,51 @@
     <t>concentration_method</t>
   </si>
   <si>
+    <t>wind_speed</t>
+  </si>
+  <si>
+    <t>SDN:P07::CFSN0038</t>
+  </si>
+  <si>
+    <t>wind_direction</t>
+  </si>
+  <si>
+    <t>SDN:P07::CFSN0036</t>
+  </si>
+  <si>
+    <t>samp_store_sol</t>
+  </si>
+  <si>
+    <t>samp_store_dur</t>
+  </si>
+  <si>
+    <t>samp_store_method_additional</t>
+  </si>
+  <si>
+    <t>stationed_sample_dur</t>
+  </si>
+  <si>
+    <t>prefilter_material</t>
+  </si>
+  <si>
+    <t>size_frac_low</t>
+  </si>
+  <si>
+    <t>µm</t>
+  </si>
+  <si>
+    <t>MixS</t>
+  </si>
+  <si>
+    <t>NERC_related</t>
+  </si>
+  <si>
     <t>expedition_id</t>
   </si>
   <si>
+    <t>SDN:W01::033</t>
+  </si>
+  <si>
     <t>user_defined</t>
   </si>
   <si>
@@ -323,39 +653,51 @@
     <t>density</t>
   </si>
   <si>
-    <t>density_unit</t>
+    <t>SDN:OG1::DENSITY</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>MIXS:0000435</t>
+    </r>
   </si>
   <si>
     <t>ammonia</t>
   </si>
   <si>
-    <t>ammonia_unit</t>
-  </si>
-  <si>
     <t>par</t>
   </si>
   <si>
-    <t>par_unit</t>
+    <t>SDN:P14::GVAR0627</t>
   </si>
   <si>
     <t>beam_attenuation</t>
   </si>
   <si>
+    <t>SDN:P01::ATTNZZ01</t>
+  </si>
+  <si>
     <t>beam_attenuation_standard_deviation</t>
   </si>
   <si>
-    <t>beam_attenuation_unit</t>
-  </si>
-  <si>
     <t>tot_inorg_nitro_to_phos_ratio</t>
   </si>
   <si>
     <t>expedition_name</t>
   </si>
   <si>
+    <t>SDN:W01::034</t>
+  </si>
+  <si>
     <t>rosette_position</t>
   </si>
   <si>
+    <t>SDN:P01::ROSPOSID</t>
+  </si>
+  <si>
     <t>collected_by</t>
   </si>
   <si>
@@ -371,21 +713,24 @@
     <t>altitude</t>
   </si>
   <si>
-    <t>altitude_unit</t>
-  </si>
-  <si>
     <t>altitude_method</t>
   </si>
   <si>
     <t>potential_temperature_C</t>
   </si>
   <si>
+    <t>SDN:S06::S0600242</t>
+  </si>
+  <si>
     <t>potential_temperature_C_standard_deviation</t>
   </si>
   <si>
     <t>percent_oxygen_sat</t>
   </si>
   <si>
+    <t>SDN:P01::OXYSZZ01</t>
+  </si>
+  <si>
     <t>percent_oxygen_sat_standard_deviation</t>
   </si>
   <si>
@@ -395,13 +740,10 @@
     <t>oxygen_solubility_standard_deviation</t>
   </si>
   <si>
-    <t>oxygen_solubility_unit</t>
-  </si>
-  <si>
     <t>sigma_theta</t>
   </si>
   <si>
-    <t>sigma_theta_unit</t>
+    <t>SDN:P07::CFSN0333</t>
   </si>
   <si>
     <t>pressure_standard_deviation</t>
@@ -416,12 +758,21 @@
     <t>decimalLongitude_standard_deviation</t>
   </si>
   <si>
+    <t>SDN:P01::ALONSD01</t>
+  </si>
+  <si>
     <t>decimalLatitude_standard_deviation</t>
   </si>
   <si>
+    <t>SDN:P01::ALATSD01</t>
+  </si>
+  <si>
     <t>ammonium_WOCE_flag</t>
   </si>
   <si>
+    <t>SDN:L27::WOCEBOTTLE_QC</t>
+  </si>
+  <si>
     <t>phosphate_WOCE_flag</t>
   </si>
   <si>
@@ -482,75 +833,78 @@
     <t>niskin_WOCE_flag</t>
   </si>
   <si>
+    <t>SDN:L27::WOCESAMPLE_QC</t>
+  </si>
+  <si>
     <t>omega_arag_method</t>
   </si>
   <si>
     <t>omega_arag</t>
   </si>
   <si>
+    <t>SDN:P01::ARGTWCAL</t>
+  </si>
+  <si>
     <t>air_temperature</t>
   </si>
   <si>
-    <t>air_temperature_unit</t>
+    <t>SDN:B39::airtemp</t>
   </si>
   <si>
     <t>air_pressure_at_sea_level</t>
   </si>
   <si>
-    <t>air_pressure_at_sea_level_unit</t>
+    <t>SDN:P07::Q9ZYSAOC</t>
   </si>
   <si>
     <t>methane</t>
   </si>
   <si>
-    <t>methane_unit</t>
-  </si>
-  <si>
     <t>synechococcus_abundance</t>
   </si>
   <si>
-    <t>synechococcus_abundance_unit</t>
+    <t>SDN:P01::P700M90E</t>
   </si>
   <si>
     <t>eukaryotic_phytoplankton_abundance</t>
   </si>
   <si>
-    <t>eukaryotic_phytoplankton_abundance_unit</t>
+    <t>SDN:P01::PHYTEXPF</t>
   </si>
   <si>
     <t>large_diatom_abundance</t>
   </si>
   <si>
-    <t>large_diatom_abundance_unit</t>
-  </si>
-  <si>
     <t>cryptophyte_abundance</t>
   </si>
   <si>
-    <t>cryptophyte_abundance_unit</t>
+    <t>SDN:P01::J79A0596</t>
   </si>
   <si>
     <t>bacteria_abundance</t>
   </si>
   <si>
-    <t>bacteria_abundance_unit</t>
+    <t>SDN:P02::BNTX</t>
   </si>
   <si>
     <t>hna_bacteria_abundance</t>
   </si>
   <si>
-    <t>hna_bacteria_abundance_unit</t>
+    <t>SDN:S25::BE006308</t>
   </si>
   <si>
     <t>lna_bacteria_abundance</t>
   </si>
   <si>
-    <t>lna_bacteria_abundance_unit</t>
+    <t>SDN:S25::BE006307</t>
   </si>
   <si>
     <t>omega_calc</t>
   </si>
   <si>
+    <t>SDN:P01::CLCTWCAL</t>
+  </si>
+  <si>
     <t>omega_calc_method</t>
   </si>
   <si>
@@ -560,133 +914,292 @@
     <t>fluor</t>
   </si>
   <si>
-    <t>fluor_unit</t>
+    <t>SDN:OD1::FLUO</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>MIXS:0000704</t>
+    </r>
   </si>
   <si>
     <t>redox_potential</t>
   </si>
   <si>
-    <t>redox_potential_unit</t>
-  </si>
-  <si>
-    <t>measurementValue</t>
+    <t>SDN:P21::MS9166</t>
+  </si>
+  <si>
+    <t>MIXS:0000182</t>
+  </si>
+  <si>
+    <t>verbatimMeasurementType</t>
   </si>
   <si>
     <t>measurementUnit</t>
   </si>
   <si>
-    <t>measurementValueID</t>
-  </si>
-  <si>
     <t>measurementRemarks</t>
   </si>
   <si>
+    <t>Expedition ID</t>
+  </si>
+  <si>
+    <t>GU19-01</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.25923/3jjh-dr85</t>
+  </si>
+  <si>
+    <t>NOAA Ship Gordon Gunter (GU), RESTORE survey  GU1901</t>
+  </si>
+  <si>
+    <t>CTD bottle number</t>
+  </si>
+  <si>
+    <t>Depth category of sample collection</t>
+  </si>
+  <si>
+    <t>Sample category</t>
+  </si>
+  <si>
+    <t>FAIRe DOI?</t>
+  </si>
+  <si>
+    <t>Natural or artificial habitat</t>
+  </si>
+  <si>
+    <t>Boolean: whether samples were taken from natural (0) or artificial (1) habitat.</t>
+  </si>
+  <si>
     <t>samp_store_temp</t>
   </si>
   <si>
+    <t>Temperature sample was stored</t>
+  </si>
+  <si>
+    <t>https://vocab.nerc.ac.uk/collection/P06/current/UPAA/</t>
+  </si>
+  <si>
+    <t>Solution sample was stored in</t>
+  </si>
+  <si>
+    <t>Duration sample was stored prior to DNA extraction</t>
+  </si>
+  <si>
+    <t>ISO 8601</t>
+  </si>
+  <si>
+    <t>https://vocab.nerc.ac.uk/collection/P06/current/TISO/</t>
+  </si>
+  <si>
+    <t>samp_store_loc</t>
+  </si>
+  <si>
+    <t>Location sample was stored</t>
+  </si>
+  <si>
+    <t>Location extracted DNA was stored</t>
+  </si>
+  <si>
+    <t>Active or passive filtration approach</t>
+  </si>
+  <si>
+    <t>Boolean: Whether water samples were collected using active (1) or passive (0) filtration approach.</t>
+  </si>
+  <si>
+    <t>Diameter of water filter</t>
+  </si>
+  <si>
+    <t>millimeters</t>
+  </si>
+  <si>
+    <t>FAIRe DOI? http://vocab.nerc.ac.uk/collection/P01/current/DSAMPA01/</t>
+  </si>
+  <si>
+    <t>http://vocab.nerc.ac.uk/collection/P06/current/UXMM/</t>
+  </si>
+  <si>
+    <t>Material of water filter</t>
+  </si>
+  <si>
+    <t>cellulose ester</t>
+  </si>
+  <si>
+    <t>Commercial names and brand of filter</t>
+  </si>
+  <si>
+    <t>prepped_samp_store_temp</t>
+  </si>
+  <si>
+    <t>Temperature prepared sample was stored prior to DNA extraction</t>
+  </si>
+  <si>
+    <t>prepped_samp_store_sol</t>
+  </si>
+  <si>
+    <t>Solution prepared sample was stored prior to DNA extraction</t>
+  </si>
+  <si>
+    <t>longmire</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1186/s13104-016-2104-5</t>
+  </si>
+  <si>
+    <t>prepped_samp_store_dur</t>
+  </si>
+  <si>
+    <t>Duration prepared sample was stored prior to DNA extraction</t>
+  </si>
+  <si>
+    <t>Date of nucleic acid extraction</t>
+  </si>
+  <si>
+    <t>nucl_acid_ext_lysis</t>
+  </si>
+  <si>
+    <t>Nucleic acid extraction lysis approach</t>
+  </si>
+  <si>
+    <t>Controlled vocabulary (physical | chemical | enzymatic | thermal | osmotic | other:)</t>
+  </si>
+  <si>
+    <t>nucl_acid_ext_sep</t>
+  </si>
+  <si>
+    <t>Nucleic acid extraction separation approach</t>
+  </si>
+  <si>
+    <t>Controlled vocabulary (column-based | magnetic beads | centrifugation | precipitation | phenol chloroform | gel electrophoresis | other:)</t>
+  </si>
+  <si>
+    <t>nucl_acid_ext_kit</t>
+  </si>
+  <si>
+    <t>Nucleic acid extraction kit</t>
+  </si>
+  <si>
+    <t>dna_cleanup_0_1</t>
+  </si>
+  <si>
+    <t>DNA cleanup</t>
+  </si>
+  <si>
+    <t>Boolean: Was the extracted DNA cleaned/purified? Yes = 1, No =0</t>
+  </si>
+  <si>
+    <t>dna_cleanup_method</t>
+  </si>
+  <si>
+    <t>DNA cleanup method</t>
+  </si>
+  <si>
+    <t>DNA concentration method</t>
+  </si>
+  <si>
+    <t>Water temperature</t>
+  </si>
+  <si>
+    <t>http://vocab.nerc.ac.uk/collection/P07/current/CFSN0335/</t>
+  </si>
+  <si>
+    <t>Chlorophyll fluorescence</t>
+  </si>
+  <si>
+    <t>micrograms per litre</t>
+  </si>
+  <si>
+    <t>http://vocab.nerc.ac.uk/collection/P01/current/CPHLMOD2/</t>
+  </si>
+  <si>
+    <t>http://vocab.nerc.ac.uk/collection/P06/current/UGPL/</t>
+  </si>
+  <si>
+    <t>Collected by WetLabs WetStar Fluorometer</t>
+  </si>
+  <si>
+    <t>Salinity</t>
+  </si>
+  <si>
+    <t>psu</t>
+  </si>
+  <si>
+    <t>http://vocab.nerc.ac.uk/collection/P01/current/ODSDM021/</t>
+  </si>
+  <si>
+    <t>http://vocab.nerc.ac.uk/collection/P06/current/PSUX/</t>
+  </si>
+  <si>
+    <t>Dissolved oxygen</t>
+  </si>
+  <si>
+    <t>http://vocab.nerc.ac.uk/collection/P06/current/UMGL/</t>
+  </si>
+  <si>
+    <t>Transmittance of the water column</t>
+  </si>
+  <si>
+    <t>percent</t>
+  </si>
+  <si>
+    <t>http://vocab.nerc.ac.uk/collection/P02/current/ATTN/</t>
+  </si>
+  <si>
+    <t>Collected by WetLabs C-Star</t>
+  </si>
+  <si>
+    <t>Density of the water column</t>
+  </si>
+  <si>
+    <t>kilograms per cubic metre</t>
+  </si>
+  <si>
+    <t>http://vocab.nerc.ac.uk/collection/P01/current/TOKGPR02/</t>
+  </si>
+  <si>
+    <t>http://vocab.nerc.ac.uk/collection/P06/current/UKMC/</t>
+  </si>
+  <si>
+    <t>eventID</t>
+  </si>
+  <si>
+    <t>occurrenceID</t>
+  </si>
+  <si>
+    <t>water_sampleA</t>
+  </si>
+  <si>
+    <t>asv1_watersampleA</t>
+  </si>
+  <si>
+    <t>temperature</t>
+  </si>
+  <si>
     <t>degC</t>
   </si>
   <si>
     <t>x11</t>
   </si>
   <si>
-    <t>doi:C</t>
-  </si>
-  <si>
-    <t>mm</t>
-  </si>
-  <si>
-    <t>good measurement</t>
-  </si>
-  <si>
-    <t>samp_size</t>
-  </si>
-  <si>
-    <t>x12</t>
-  </si>
-  <si>
-    <t>doi:Volume</t>
-  </si>
-  <si>
-    <t>bad measurement</t>
-  </si>
-  <si>
-    <t>nucl_acid_ext_sep</t>
-  </si>
-  <si>
-    <t>phenol chloroform</t>
-  </si>
-  <si>
-    <t>DOI:mag</t>
-  </si>
-  <si>
-    <t>hi</t>
+    <t>water_sampleB</t>
+  </si>
+  <si>
+    <t>asv1_watersampleB</t>
   </si>
   <si>
     <t>env_broad_scale</t>
   </si>
   <si>
-    <t>marine biome</t>
+    <t xml:space="preserve">marine biome </t>
   </si>
   <si>
     <t>x22</t>
   </si>
   <si>
     <t>[ENVO:00000447]</t>
-  </si>
-  <si>
-    <t>DOI:exampleURL</t>
-  </si>
-  <si>
-    <t>hello</t>
-  </si>
-  <si>
-    <t>env_local_scale</t>
-  </si>
-  <si>
-    <t>marine mesopelagic zone</t>
-  </si>
-  <si>
-    <t>[ENVO:00000213]</t>
-  </si>
-  <si>
-    <t>DOI:anotherExample</t>
-  </si>
-  <si>
-    <t>concentration</t>
-  </si>
-  <si>
-    <t>x2121</t>
-  </si>
-  <si>
-    <t>doi:Concentration</t>
-  </si>
-  <si>
-    <t>collected after freezing</t>
-  </si>
-  <si>
-    <t>eventID</t>
-  </si>
-  <si>
-    <t>occurrenceID</t>
-  </si>
-  <si>
-    <t>water_sampleA</t>
-  </si>
-  <si>
-    <t>asv1_watersampleA</t>
-  </si>
-  <si>
-    <t>temperature</t>
-  </si>
-  <si>
-    <t>water_sampleB</t>
-  </si>
-  <si>
-    <t>asv1_watersampleB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">marine biome </t>
   </si>
   <si>
     <t xml:space="preserve">plant biome </t>
@@ -825,7 +1338,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="14">
+  <fonts count="23">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -847,6 +1360,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11.0"/>
+      <color rgb="FF0000FF"/>
+      <name val="&quot;Helvetica Neue&quot;"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="&quot;Helvetica Neue&quot;"/>
+    </font>
+    <font>
       <b/>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
@@ -866,6 +1390,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11.0"/>
+      <color rgb="FF0000FF"/>
+      <name val="&quot;Helvetica Neue&quot;"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+    </font>
+    <font>
       <b/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -877,16 +1415,40 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12.0"/>
       <color rgb="FF000000"/>
+      <name val="System-ui"/>
+    </font>
+    <font>
+      <sz val="10.0"/>
+      <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12.0"/>
+      <color rgb="FF333333"/>
+      <name val="-apple-system"/>
+    </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="10.0"/>
+      <color rgb="FF0000FF"/>
     </font>
     <font>
       <color theme="1"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <color rgb="FF0000FF"/>
     </font>
     <font>
       <b/>
@@ -898,7 +1460,7 @@
       <color rgb="FF000000"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -919,6 +1481,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFCDD8DE"/>
+        <bgColor rgb="FFCDD8DE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFE0FFFF"/>
         <bgColor rgb="FFE0FFFF"/>
       </patternFill>
@@ -930,7 +1504,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="36">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -940,61 +1514,93 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="top"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="4" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="16" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -1230,8 +1836,9 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="21.88"/>
-    <col customWidth="1" min="2" max="2" width="20.25"/>
-    <col customWidth="1" min="3" max="4" width="23.88"/>
+    <col customWidth="1" min="2" max="4" width="20.25"/>
+    <col customWidth="1" min="5" max="5" width="23.88"/>
+    <col customWidth="1" min="6" max="6" width="21.75"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1241,130 +1848,210 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3"/>
+      <c r="B2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="s">
-        <v>8</v>
+      <c r="A3" s="7" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="s">
-        <v>9</v>
-      </c>
+      <c r="A4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="s">
-        <v>10</v>
+      <c r="A5" s="8" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="5" t="s">
-        <v>11</v>
+      <c r="A6" s="8" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="5" t="s">
-        <v>12</v>
+      <c r="A7" s="8" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="5" t="s">
-        <v>13</v>
+      <c r="A8" s="8" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="6" t="s">
-        <v>14</v>
+      <c r="A9" s="9" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>16</v>
+      <c r="A10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="6" t="s">
-        <v>17</v>
+      <c r="A11" s="9" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="6" t="s">
-        <v>18</v>
+      <c r="A12" s="9" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="6" t="s">
-        <v>19</v>
+      <c r="A13" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
     <row r="16">
-      <c r="A16" s="6" t="s">
-        <v>22</v>
+      <c r="A16" s="9" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="6" t="s">
-        <v>27</v>
+    </row>
+    <row r="26">
+      <c r="A26" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <mergeCells count="2">
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B22:E22"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink r:id="rId2" ref="B2"/>
+    <hyperlink r:id="rId3" ref="F2"/>
+    <hyperlink r:id="rId4" ref="B4"/>
+    <hyperlink r:id="rId5" ref="B21"/>
+    <hyperlink r:id="rId6" ref="B22"/>
+  </hyperlinks>
+  <drawing r:id="rId7"/>
+  <legacyDrawing r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -1374,474 +2061,767 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="38.0"/>
-    <col customWidth="1" min="2" max="2" width="20.63"/>
-    <col customWidth="1" min="3" max="3" width="18.25"/>
-    <col customWidth="1" min="4" max="4" width="21.38"/>
-    <col customWidth="1" min="5" max="5" width="18.25"/>
+    <col customWidth="1" min="2" max="2" width="28.63"/>
+    <col customWidth="1" min="3" max="4" width="18.25"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="C1" s="11" t="s">
         <v>4</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>29</v>
+      <c r="A2" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="8" t="s">
-        <v>30</v>
+      <c r="A3" s="14" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="7" t="s">
-        <v>31</v>
+      <c r="A4" s="12" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="6" t="s">
-        <v>32</v>
+      <c r="A5" s="9" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="6" t="s">
-        <v>33</v>
+      <c r="A6" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="9" t="s">
-        <v>34</v>
+      <c r="A7" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="10" t="s">
-        <v>35</v>
+      <c r="A8" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="10" t="s">
-        <v>36</v>
-      </c>
+      <c r="A9" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="17"/>
     </row>
     <row r="10">
-      <c r="A10" s="10" t="s">
-        <v>37</v>
+      <c r="A10" s="18" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="10" t="s">
-        <v>38</v>
+      <c r="A11" s="8" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="10" t="s">
-        <v>39</v>
+      <c r="A12" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="11" t="s">
-        <v>40</v>
+      <c r="A13" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="10" t="s">
-        <v>41</v>
+      <c r="A14" s="16" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="5" t="s">
-        <v>42</v>
+      <c r="A15" s="16" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="12" t="s">
-        <v>43</v>
+      <c r="A16" s="16" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="10" t="s">
-        <v>44</v>
+      <c r="A17" s="16" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="10" t="s">
-        <v>45</v>
+      <c r="A18" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="10" t="s">
-        <v>46</v>
+      <c r="A19" s="16" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="10" t="s">
-        <v>47</v>
+      <c r="A20" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="10" t="s">
-        <v>48</v>
+      <c r="A21" s="16" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="10" t="s">
-        <v>49</v>
+      <c r="A22" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="10" t="s">
-        <v>50</v>
+      <c r="A23" s="16" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="10" t="s">
-        <v>51</v>
+      <c r="A24" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="10" t="s">
-        <v>52</v>
+      <c r="A25" s="16" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="10" t="s">
-        <v>53</v>
+      <c r="A26" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="10" t="s">
-        <v>54</v>
+      <c r="A27" s="18" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="10" t="s">
-        <v>55</v>
+      <c r="A28" s="20" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="10" t="s">
-        <v>56</v>
+      <c r="A29" s="20" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="10" t="s">
-        <v>57</v>
+      <c r="A30" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="10" t="s">
-        <v>58</v>
-      </c>
+      <c r="A31" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C31" s="11"/>
     </row>
     <row r="32">
-      <c r="A32" s="10" t="s">
-        <v>59</v>
+      <c r="A32" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C32" s="11"/>
+      <c r="G32" s="10" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="10" t="s">
-        <v>60</v>
+      <c r="A33" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C33" s="11"/>
+      <c r="G33" s="10" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="11" t="s">
-        <v>61</v>
+      <c r="A34" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C34" s="11"/>
+      <c r="G34" s="10" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="13" t="s">
-        <v>62</v>
+      <c r="A35" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C35" s="11"/>
+      <c r="G35" s="10" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="13" t="s">
-        <v>63</v>
+      <c r="A36" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" s="11"/>
+      <c r="G36" s="10" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="5" t="s">
-        <v>64</v>
+      <c r="A37" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C37" s="11"/>
+      <c r="G37" s="10" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="5" t="s">
-        <v>65</v>
+      <c r="A38" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C38" s="11"/>
+      <c r="G38" s="10" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="11" t="s">
-        <v>66</v>
+      <c r="A39" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C39" s="11"/>
+      <c r="G39" s="10" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="11" t="s">
-        <v>67</v>
+      <c r="A40" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C40" s="11"/>
+      <c r="G40" s="10" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="11" t="s">
-        <v>68</v>
+      <c r="A41" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C41" s="11"/>
+      <c r="G41" s="10" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="14" t="s">
-        <v>69</v>
+      <c r="A42" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C42" s="11"/>
+      <c r="G42" s="10" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="14" t="s">
-        <v>70</v>
+      <c r="A43" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C43" s="11"/>
+      <c r="G43" s="10" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="14" t="s">
-        <v>71</v>
+      <c r="A44" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="B44" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C44" s="11"/>
+      <c r="G44" s="10" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="14" t="s">
-        <v>72</v>
+      <c r="A45" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C45" s="11"/>
+      <c r="G45" s="10" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="14" t="s">
-        <v>73</v>
+      <c r="A46" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C46" s="11"/>
+      <c r="G46" s="10" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="14" t="s">
-        <v>74</v>
+      <c r="A47" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="B47" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C47" s="11"/>
+      <c r="G47" s="10" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="14" t="s">
-        <v>75</v>
+      <c r="A48" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="B48" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C48" s="11"/>
+      <c r="G48" s="10" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="14" t="s">
-        <v>76</v>
+      <c r="A49" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="B49" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C49" s="11"/>
+      <c r="G49" s="10" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="14" t="s">
-        <v>77</v>
+      <c r="A50" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="B50" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C50" s="11"/>
+      <c r="G50" s="10" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="14" t="s">
-        <v>78</v>
+      <c r="A51" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="B51" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C51" s="11"/>
+      <c r="G51" s="10" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="14" t="s">
-        <v>79</v>
+      <c r="A52" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="B52" s="13" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="14" t="s">
-        <v>80</v>
+      <c r="A53" s="18" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="14" t="s">
-        <v>81</v>
+      <c r="A54" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="14" t="s">
-        <v>82</v>
+      <c r="A55" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="14" t="s">
-        <v>83</v>
+      <c r="A56" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G56" s="5" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="14" t="s">
-        <v>84</v>
+      <c r="A57" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="14" t="s">
-        <v>85</v>
+      <c r="A58" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G58" s="5" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="14" t="s">
-        <v>86</v>
+      <c r="A59" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G59" s="5" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="11" t="s">
-        <v>87</v>
+      <c r="A60" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="10" t="s">
-        <v>88</v>
+      <c r="A61" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F61" s="22"/>
+      <c r="G61" s="23" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="10" t="s">
-        <v>89</v>
+      <c r="A62" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B62" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="10" t="s">
-        <v>90</v>
+      <c r="A63" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="10" t="s">
-        <v>91</v>
+      <c r="A64" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="10" t="s">
-        <v>92</v>
+      <c r="A65" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="10" t="s">
-        <v>93</v>
+      <c r="A66" s="16" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="10" t="s">
-        <v>94</v>
+      <c r="A67" s="24" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="10" t="s">
-        <v>95</v>
+      <c r="A68" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B68" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F68" s="15" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="10" t="s">
-        <v>96</v>
+      <c r="A69" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F69" s="23" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="10" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" s="10" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" s="10" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" s="10" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" s="10" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" s="10" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" s="10" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" s="10" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" s="10" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" s="10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" s="10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" s="10" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" s="10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" s="15" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" s="10" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" s="10" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" s="10" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" s="10" t="s">
-        <v>115</v>
-      </c>
+      <c r="A70" s="16"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <mergeCells count="21">
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="G51:H51"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="G44:H44"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink r:id="rId2" ref="B2"/>
+    <hyperlink r:id="rId3" ref="B6"/>
+    <hyperlink r:id="rId4" ref="F6"/>
+    <hyperlink r:id="rId5" ref="B8"/>
+    <hyperlink r:id="rId6" ref="B9"/>
+    <hyperlink r:id="rId7" ref="B12"/>
+    <hyperlink r:id="rId8" ref="B13"/>
+    <hyperlink r:id="rId9" ref="B20"/>
+    <hyperlink r:id="rId10" ref="D20"/>
+    <hyperlink r:id="rId11" ref="B22"/>
+    <hyperlink r:id="rId12" ref="B26"/>
+    <hyperlink r:id="rId13" ref="B30"/>
+    <hyperlink r:id="rId14" ref="B31"/>
+    <hyperlink r:id="rId15" ref="B32"/>
+    <hyperlink r:id="rId16" ref="G32"/>
+    <hyperlink r:id="rId17" ref="B33"/>
+    <hyperlink r:id="rId18" ref="G33"/>
+    <hyperlink r:id="rId19" ref="B34"/>
+    <hyperlink r:id="rId20" ref="G34"/>
+    <hyperlink r:id="rId21" ref="B35"/>
+    <hyperlink r:id="rId22" ref="G35"/>
+    <hyperlink r:id="rId23" ref="B36"/>
+    <hyperlink r:id="rId24" ref="G36"/>
+    <hyperlink r:id="rId25" ref="B37"/>
+    <hyperlink r:id="rId26" ref="G37"/>
+    <hyperlink r:id="rId27" ref="B38"/>
+    <hyperlink r:id="rId28" ref="G38"/>
+    <hyperlink r:id="rId29" ref="B39"/>
+    <hyperlink r:id="rId30" ref="G39"/>
+    <hyperlink r:id="rId31" ref="B40"/>
+    <hyperlink r:id="rId32" ref="G40"/>
+    <hyperlink r:id="rId33" ref="B41"/>
+    <hyperlink r:id="rId34" ref="G41"/>
+    <hyperlink r:id="rId35" ref="B42"/>
+    <hyperlink r:id="rId36" ref="G42"/>
+    <hyperlink r:id="rId37" ref="B43"/>
+    <hyperlink r:id="rId38" ref="G43"/>
+    <hyperlink r:id="rId39" ref="B44"/>
+    <hyperlink r:id="rId40" ref="G44"/>
+    <hyperlink r:id="rId41" ref="B45"/>
+    <hyperlink r:id="rId42" ref="G45"/>
+    <hyperlink r:id="rId43" ref="B46"/>
+    <hyperlink r:id="rId44" ref="G46"/>
+    <hyperlink r:id="rId45" ref="B47"/>
+    <hyperlink r:id="rId46" ref="G47"/>
+    <hyperlink r:id="rId47" ref="B48"/>
+    <hyperlink r:id="rId48" ref="G48"/>
+    <hyperlink r:id="rId49" ref="B49"/>
+    <hyperlink r:id="rId50" ref="G49"/>
+    <hyperlink r:id="rId51" ref="B50"/>
+    <hyperlink r:id="rId52" ref="G50"/>
+    <hyperlink r:id="rId53" ref="B51"/>
+    <hyperlink r:id="rId54" ref="G51"/>
+    <hyperlink r:id="rId55" ref="B52"/>
+    <hyperlink r:id="rId56" ref="B54"/>
+    <hyperlink r:id="rId57" ref="B55"/>
+    <hyperlink r:id="rId58" ref="G56"/>
+    <hyperlink r:id="rId59" ref="G58"/>
+    <hyperlink r:id="rId60" ref="G59"/>
+    <hyperlink r:id="rId61" ref="G61"/>
+    <hyperlink r:id="rId62" ref="B62"/>
+    <hyperlink r:id="rId63" ref="B63"/>
+    <hyperlink r:id="rId64" ref="B64"/>
+    <hyperlink r:id="rId65" ref="B65"/>
+    <hyperlink r:id="rId66" ref="B68"/>
+    <hyperlink r:id="rId67" ref="F68"/>
+    <hyperlink r:id="rId68" ref="B69"/>
+    <hyperlink r:id="rId69" ref="F69"/>
+  </hyperlinks>
+  <drawing r:id="rId70"/>
+  <legacyDrawing r:id="rId71"/>
 </worksheet>
 </file>
 
@@ -1851,153 +2831,501 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1.0" ySplit="1.0" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="B1" sqref="B1" pane="topRight"/>
+      <selection activeCell="A2" sqref="A2" pane="bottomLeft"/>
+      <selection activeCell="B2" sqref="B2" pane="bottomRight"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="22.0"/>
-    <col customWidth="1" min="2" max="2" width="21.13"/>
-    <col customWidth="1" min="3" max="3" width="19.25"/>
-    <col customWidth="1" min="4" max="4" width="21.63"/>
-    <col customWidth="1" min="5" max="6" width="19.0"/>
+    <col customWidth="1" min="1" max="2" width="22.0"/>
+    <col customWidth="1" min="3" max="3" width="21.13"/>
+    <col customWidth="1" min="4" max="4" width="19.25"/>
+    <col customWidth="1" min="5" max="5" width="21.63"/>
+    <col customWidth="1" min="6" max="7" width="19.0"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="D1" s="16" t="s">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>119</v>
+      <c r="F1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>123</v>
+      <c r="A2" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="B6" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="F17" s="27" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="G18" s="15" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="B20" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="G26" s="15" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="B7" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>147</v>
+      <c r="B27" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="E27" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="G27" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="G28" s="15" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G29" s="15" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="G31" s="15" t="s">
+        <v>217</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <hyperlinks>
+    <hyperlink r:id="rId2" ref="E2"/>
+    <hyperlink r:id="rId3" ref="F2"/>
+    <hyperlink r:id="rId4" ref="G7"/>
+    <hyperlink r:id="rId5" ref="G9"/>
+    <hyperlink r:id="rId6" ref="G13"/>
+    <hyperlink r:id="rId7" ref="G16"/>
+    <hyperlink r:id="rId8" ref="F17"/>
+    <hyperlink r:id="rId9" ref="G18"/>
+    <hyperlink r:id="rId10" ref="G19"/>
+    <hyperlink r:id="rId11" ref="E26"/>
+    <hyperlink r:id="rId12" ref="G26"/>
+    <hyperlink r:id="rId13" ref="E27"/>
+    <hyperlink r:id="rId14" ref="G27"/>
+    <hyperlink r:id="rId15" ref="E28"/>
+    <hyperlink r:id="rId16" ref="G28"/>
+    <hyperlink r:id="rId17" ref="G29"/>
+    <hyperlink r:id="rId18" ref="E30"/>
+    <hyperlink r:id="rId19" ref="E31"/>
+    <hyperlink r:id="rId20" ref="G31"/>
+  </hyperlinks>
+  <drawing r:id="rId21"/>
+  <legacyDrawing r:id="rId22"/>
 </worksheet>
 </file>
 
@@ -2023,147 +3351,147 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>148</v>
+        <v>218</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>149</v>
+        <v>219</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="F1" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="H1" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="16" t="s">
-        <v>119</v>
+      <c r="G1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="D2" s="3">
+      <c r="A2" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="D2" s="4">
         <v>18.0</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>122</v>
+      <c r="E2" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="D3" s="3">
+      <c r="A3" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="D3" s="4">
         <v>19.0</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>122</v>
+      <c r="E3" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="4">
-      <c r="C4" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>155</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>137</v>
+      <c r="C4" s="31" t="s">
+        <v>227</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>228</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="5">
-      <c r="C5" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>156</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>157</v>
+      <c r="C5" s="31" t="s">
+        <v>227</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>231</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="6">
-      <c r="C6" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>159</v>
-      </c>
-      <c r="F6" s="20" t="s">
-        <v>160</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>161</v>
+      <c r="C6" s="31" t="s">
+        <v>233</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>234</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="7">
-      <c r="C7" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="F7" s="20" t="s">
-        <v>160</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>161</v>
+      <c r="C7" s="31" t="s">
+        <v>233</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="8">
-      <c r="C8" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>165</v>
+      <c r="C8" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="9">
-      <c r="C9" s="3" t="s">
-        <v>20</v>
+      <c r="C9" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="3"/>
+      <c r="A10" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2186,174 +3514,174 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="15" t="s">
-        <v>166</v>
+      <c r="A1" s="24" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>167</v>
+      <c r="A2" s="4" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>168</v>
+      <c r="A4" s="4" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="s">
-        <v>169</v>
+      <c r="A6" s="4" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="s">
-        <v>170</v>
+      <c r="A7" s="4" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="s">
-        <v>171</v>
+      <c r="A8" s="4" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="3" t="s">
-        <v>172</v>
+      <c r="A10" s="4" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="3" t="s">
-        <v>173</v>
+      <c r="A11" s="4" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="12">
-      <c r="B12" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="H12" s="21" t="s">
-        <v>175</v>
+      <c r="B12" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="H12" s="33" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="13">
-      <c r="C13" s="3" t="s">
-        <v>176</v>
+      <c r="C13" s="4" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="14">
-      <c r="C14" s="3" t="s">
-        <v>177</v>
+      <c r="C14" s="4" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="15">
-      <c r="C15" s="3" t="s">
-        <v>178</v>
+      <c r="C15" s="4" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="16">
-      <c r="C16" s="3" t="s">
-        <v>179</v>
+      <c r="C16" s="4" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="17">
-      <c r="C17" s="3"/>
+      <c r="C17" s="4"/>
     </row>
     <row r="18">
-      <c r="C18" s="3" t="s">
-        <v>180</v>
+      <c r="C18" s="4" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="19">
-      <c r="C19" s="3" t="s">
-        <v>181</v>
+      <c r="C19" s="4" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="21">
-      <c r="C21" s="3" t="s">
-        <v>182</v>
+      <c r="C21" s="4" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="22">
-      <c r="D22" s="3" t="s">
-        <v>183</v>
+      <c r="D22" s="4" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="24">
-      <c r="C24" s="3" t="s">
-        <v>184</v>
+      <c r="C24" s="4" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="25">
-      <c r="D25" s="3" t="s">
-        <v>185</v>
+      <c r="D25" s="4" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="28">
-      <c r="C28" s="3" t="s">
-        <v>186</v>
+      <c r="C28" s="4" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="29">
-      <c r="C29" s="3" t="s">
-        <v>187</v>
+      <c r="C29" s="4" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="30">
-      <c r="C30" s="3" t="s">
-        <v>188</v>
+      <c r="C30" s="4" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="31">
-      <c r="D31" s="3" t="s">
-        <v>189</v>
+      <c r="D31" s="4" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="32">
-      <c r="D32" s="3" t="s">
-        <v>190</v>
+      <c r="D32" s="4" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="33">
-      <c r="C33" s="3" t="s">
-        <v>191</v>
+      <c r="C33" s="4" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="34">
-      <c r="D34" s="3" t="s">
-        <v>192</v>
+      <c r="D34" s="4" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="35">
-      <c r="C35" s="3" t="s">
-        <v>193</v>
+      <c r="C35" s="4" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="36">
-      <c r="D36" s="3" t="s">
-        <v>194</v>
+      <c r="D36" s="4" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="3" t="s">
-        <v>195</v>
+      <c r="A39" s="4" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="22" t="s">
-        <v>196</v>
+      <c r="A41" s="34" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="23" t="s">
-        <v>197</v>
+      <c r="A42" s="35" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="20" t="s">
-        <v>198</v>
+      <c r="A43" s="15" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="3" t="s">
-        <v>199</v>
+      <c r="A45" s="4" t="s">
+        <v>274</v>
       </c>
     </row>
   </sheetData>

</xml_diff>